<commit_message>
29441 Project > Timesheet > Detail > Export Invoice For Tax
</commit_message>
<xml_diff>
--- a/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/InvoiceUserTemplateForTax.xlsx
+++ b/aspnet-core/src/ProjectManagement.Web.Host/wwwroot/template/InvoiceUserTemplateForTax.xlsx
@@ -231,7 +231,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00;;"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00;;\-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="8"/>
       <color theme="3"/>
@@ -380,6 +380,13 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="3"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -471,7 +478,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -630,18 +637,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -728,7 +738,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -1917,16 +1927,16 @@
       </c>
     </row>
     <row r="3" spans="2:10" ht="24" customHeight="1">
-      <c r="B3" s="62">
+      <c r="B3" s="63">
         <v>44015</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="67">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="68">
         <f>InvoiceTotal</f>
         <v>0</v>
       </c>
-      <c r="F3" s="67"/>
+      <c r="F3" s="68"/>
       <c r="G3" s="11" t="s">
         <v>3</v>
       </c>
@@ -1937,49 +1947,49 @@
       </c>
       <c r="C4" s="14"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
       <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:10">
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64" t="s">
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="64"/>
+      <c r="F6" s="65"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66" t="s">
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="66"/>
+      <c r="F7" s="67"/>
     </row>
     <row r="8" spans="2:10">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="55"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
       <c r="F9" s="19"/>
     </row>
     <row r="10" spans="2:10" ht="12.75" customHeight="1">
@@ -2065,11 +2075,11 @@
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
-      <c r="E19" s="58" t="str">
+      <c r="E19" s="59" t="str">
         <f>REPT(CompanySetup_YourCurrencyAbbreviation,LEN(CompanySetup_YourCurrencyAbbreviation)&gt;0)&amp;" TOTAL"</f>
         <v>USD TOTAL</v>
       </c>
-      <c r="F19" s="60">
+      <c r="F19" s="61">
         <f>F17+F18</f>
         <v>0</v>
       </c>
@@ -2078,8 +2088,8 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="61"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="62"/>
     </row>
     <row r="22" spans="2:9" ht="15">
       <c r="B22" s="40" t="s">
@@ -2159,11 +2169,11 @@
       <c r="I29" s="45"/>
     </row>
     <row r="30" spans="2:9" ht="27" customHeight="1">
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
       <c r="I30" s="45"/>
     </row>
   </sheetData>
@@ -2365,8 +2375,8 @@
       <c r="C21" s="10"/>
     </row>
     <row r="22" spans="2:3" ht="18.75" customHeight="1">
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
@@ -2388,50 +2398,50 @@
   <dimension ref="B1:E20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="54" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="53" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="64" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="34.5" customHeight="1">
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="2:5" ht="22.5" customHeight="1">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="55" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="9.75" customHeight="1">
-      <c r="B3" s="9"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="52"/>
     </row>
     <row r="4" spans="2:5" ht="18.75" customHeight="1" thickBot="1">
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
     </row>
     <row r="5" spans="2:5" ht="18.75" customHeight="1" thickTop="1"/>
     <row r="20" ht="9.75" customHeight="1"/>

</xml_diff>